<commit_message>
Updated plotting for Initial conditions
</commit_message>
<xml_diff>
--- a/models/erie_tfv_aed_2013_ver012_rev0/BCs/IC/IC_Plotting_Information.xlsx
+++ b/models/erie_tfv_aed_2013_ver012_rev0/BCs/IC/IC_Plotting_Information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\Lake-Erie\models\erie_tfv_aed_2013_ver012_rev0\BCs\IC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EBB9D3-C533-48C5-A270-5E8816B1398C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEEC2E5-89B6-41F1-A512-950409E9BEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1830" windowWidth="21600" windowHeight="11385" xr2:uid="{126C559C-A826-4DEE-8514-A272FB6B47D5}"/>
+    <workbookView xWindow="7800" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{126C559C-A826-4DEE-8514-A272FB6B47D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,6 +671,9 @@
         <f>32/1000</f>
         <v>3.2000000000000001E-2</v>
       </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -698,6 +701,9 @@
         <f>14/1000</f>
         <v>1.4E-2</v>
       </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -710,6 +716,9 @@
         <f>14/1000</f>
         <v>1.4E-2</v>
       </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -749,6 +758,9 @@
         <f>12/1000</f>
         <v>1.2E-2</v>
       </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -776,6 +788,9 @@
         <f>14/1000</f>
         <v>1.4E-2</v>
       </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -802,6 +817,9 @@
       <c r="C21">
         <f>31/1000</f>
         <v>3.1E-2</v>
+      </c>
+      <c r="D21">
+        <v>0.03</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>